<commit_message>
Logistica, LASSO, Ridge, Random Foredt
</commit_message>
<xml_diff>
--- a/Projeto Final - Entrega 1.xlsx
+++ b/Projeto Final - Entrega 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/147f45201b263114/Documentos/Insper/Pos graduacao/2 Trimestre/APRENDIZAGEM ESTATÍSTICA DE MÁQUINA II/Projeto Final/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/422c37a5e5dc8557/Insper/tri_2/estatistica_2/Projeto_final/Projeto_Final_AEMII/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{02507077-C700-4B1E-B9A9-025ABF14F3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E2933F0-9016-4483-8C80-2A57E891C014}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{02507077-C700-4B1E-B9A9-025ABF14F3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0DD68F6-8600-4F4F-8E43-98BA0C9178C6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{38578D12-16BC-486B-9148-65477D577933}"/>
+    <workbookView xWindow="22932" yWindow="-4176" windowWidth="23256" windowHeight="12456" xr2:uid="{38578D12-16BC-486B-9148-65477D577933}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -103,128 +103,128 @@
 Os modelos que vão ser feitos serão Regressão Logística, Floresta Aleatória, Boosting, Lasso, Ridge e Rede Neural</t>
   </si>
   <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>dbl</t>
+  </si>
+  <si>
+    <t>Kidhome</t>
+  </si>
+  <si>
+    <t>Teenhome</t>
+  </si>
+  <si>
+    <t>Recency</t>
+  </si>
+  <si>
+    <t>MntWines</t>
+  </si>
+  <si>
+    <t>MntFruits</t>
+  </si>
+  <si>
+    <t>MntMeatProducts</t>
+  </si>
+  <si>
+    <t>MntFishProducts</t>
+  </si>
+  <si>
+    <t>MntSweetProducts</t>
+  </si>
+  <si>
+    <t>MntGoldProds</t>
+  </si>
+  <si>
+    <t>NumDealsPurchases</t>
+  </si>
+  <si>
+    <t>NumWebPurchases</t>
+  </si>
+  <si>
+    <t>NumCatalogPurchases</t>
+  </si>
+  <si>
+    <t>NumStorePurchases</t>
+  </si>
+  <si>
+    <t>NumWebVisitsMonth</t>
+  </si>
+  <si>
+    <t>AcceptedCmp3</t>
+  </si>
+  <si>
+    <t>AcceptedCmp4</t>
+  </si>
+  <si>
+    <t>AcceptedCmp5</t>
+  </si>
+  <si>
+    <t>AcceptedCmp1</t>
+  </si>
+  <si>
+    <t>AcceptedCmp2</t>
+  </si>
+  <si>
+    <t>Complain</t>
+  </si>
+  <si>
+    <t>Z_CostContact</t>
+  </si>
+  <si>
+    <t>Z_Revenue</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Customer_Days</t>
+  </si>
+  <si>
+    <t>marital_Divorced</t>
+  </si>
+  <si>
+    <t>marital_Married</t>
+  </si>
+  <si>
+    <t>marital_Single</t>
+  </si>
+  <si>
+    <t>marital_Together</t>
+  </si>
+  <si>
+    <t>marital_Widow</t>
+  </si>
+  <si>
+    <t>education_2n Cycle</t>
+  </si>
+  <si>
+    <t>education_Basic</t>
+  </si>
+  <si>
+    <t>education_Graduation</t>
+  </si>
+  <si>
+    <t>education_Master</t>
+  </si>
+  <si>
+    <t>education_PhD</t>
+  </si>
+  <si>
+    <t>MntTotal</t>
+  </si>
+  <si>
+    <t>MntRegularProds</t>
+  </si>
+  <si>
+    <t>AcceptedCmpOverall</t>
+  </si>
+  <si>
     <t>Os mesmos tratamentos da análise supervisionada, e para o método de KMeans, será retirada as colunas de variáveis categóricas.
-Serão feitos os modelos de PCA e KMeans</t>
-  </si>
-  <si>
-    <t>Income</t>
-  </si>
-  <si>
-    <t>dbl</t>
-  </si>
-  <si>
-    <t>Kidhome</t>
-  </si>
-  <si>
-    <t>Teenhome</t>
-  </si>
-  <si>
-    <t>Recency</t>
-  </si>
-  <si>
-    <t>MntWines</t>
-  </si>
-  <si>
-    <t>MntFruits</t>
-  </si>
-  <si>
-    <t>MntMeatProducts</t>
-  </si>
-  <si>
-    <t>MntFishProducts</t>
-  </si>
-  <si>
-    <t>MntSweetProducts</t>
-  </si>
-  <si>
-    <t>MntGoldProds</t>
-  </si>
-  <si>
-    <t>NumDealsPurchases</t>
-  </si>
-  <si>
-    <t>NumWebPurchases</t>
-  </si>
-  <si>
-    <t>NumCatalogPurchases</t>
-  </si>
-  <si>
-    <t>NumStorePurchases</t>
-  </si>
-  <si>
-    <t>NumWebVisitsMonth</t>
-  </si>
-  <si>
-    <t>AcceptedCmp3</t>
-  </si>
-  <si>
-    <t>AcceptedCmp4</t>
-  </si>
-  <si>
-    <t>AcceptedCmp5</t>
-  </si>
-  <si>
-    <t>AcceptedCmp1</t>
-  </si>
-  <si>
-    <t>AcceptedCmp2</t>
-  </si>
-  <si>
-    <t>Complain</t>
-  </si>
-  <si>
-    <t>Z_CostContact</t>
-  </si>
-  <si>
-    <t>Z_Revenue</t>
-  </si>
-  <si>
-    <t>Response</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Customer_Days</t>
-  </si>
-  <si>
-    <t>marital_Divorced</t>
-  </si>
-  <si>
-    <t>marital_Married</t>
-  </si>
-  <si>
-    <t>marital_Single</t>
-  </si>
-  <si>
-    <t>marital_Together</t>
-  </si>
-  <si>
-    <t>marital_Widow</t>
-  </si>
-  <si>
-    <t>education_2n Cycle</t>
-  </si>
-  <si>
-    <t>education_Basic</t>
-  </si>
-  <si>
-    <t>education_Graduation</t>
-  </si>
-  <si>
-    <t>education_Master</t>
-  </si>
-  <si>
-    <t>education_PhD</t>
-  </si>
-  <si>
-    <t>MntTotal</t>
-  </si>
-  <si>
-    <t>MntRegularProds</t>
-  </si>
-  <si>
-    <t>AcceptedCmpOverall</t>
+Serão feitos os modelos de KMeans</t>
   </si>
 </sst>
 </file>
@@ -334,11 +334,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -863,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E86E8862-2465-4932-9384-C94448F29E51}">
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -955,15 +955,15 @@
         <v>15</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -977,431 +977,431 @@
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="10" t="s">
+      <c r="A12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+      <c r="B13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
+      <c r="B14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
+      <c r="B15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
+      <c r="B16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+      <c r="B17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
+      <c r="B18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
+      <c r="B19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
+      <c r="B20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
+      <c r="B21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+      <c r="B22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
+      <c r="B23" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+      <c r="B24" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
+      <c r="B25" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
+      <c r="B26" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
+      <c r="B27" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="10" t="s">
+      <c r="B28" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
+      <c r="B29" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="s">
+      <c r="B30" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
+      <c r="B31" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
+      <c r="B32" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
+      <c r="B33" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="s">
+      <c r="B34" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="s">
+      <c r="B35" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
+      <c r="B36" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="10" t="s">
+      <c r="B37" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C37" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="10" t="s">
+      <c r="B38" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="10" t="s">
+      <c r="B39" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C39" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="10" t="s">
+      <c r="B40" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C40" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="10" t="s">
+      <c r="B41" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C41" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="10" t="s">
+      <c r="B42" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B42" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C42" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="10" t="s">
+      <c r="B43" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B43" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C43" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="10" t="s">
+      <c r="B44" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B44" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="10" t="s">
+      <c r="B45" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B45" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C45" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="10" t="s">
+      <c r="B46" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B46" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C46" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="10" t="s">
+      <c r="B47" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B47" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C47" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="10" t="s">
+      <c r="B48" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B48" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C48" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="10" t="s">
+      <c r="B49" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B49" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C49" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C50" s="10">
+      <c r="B50" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="9">
         <v>0</v>
       </c>
     </row>

</xml_diff>